<commit_message>
WIP: update .xlsx dataset
</commit_message>
<xml_diff>
--- a/data/coil_stat.xlsx
+++ b/data/coil_stat.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\python\coil-report\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="96" windowWidth="22800" windowHeight="9312"/>
+    <workbookView xWindow="90" yWindow="90" windowWidth="22800" windowHeight="9315"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="255">
   <si>
     <t>file</t>
   </si>
@@ -776,13 +781,19 @@
   </si>
   <si>
     <t>V810</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -874,7 +885,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -906,9 +917,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,6 +952,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1115,30 +1128,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K376"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H225" sqref="H225"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1172,8 +1185,11 @@
       <c r="K1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1202,7 +1218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -1231,7 +1247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -1260,7 +1276,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -1289,7 +1305,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -1318,7 +1334,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -1347,7 +1363,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -1376,7 +1392,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -1405,7 +1421,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -1434,7 +1450,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -1463,7 +1479,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>227</v>
       </c>
@@ -1492,7 +1508,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>227</v>
       </c>
@@ -1518,7 +1534,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>230</v>
       </c>
@@ -1547,7 +1563,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -1573,7 +1589,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>229</v>
       </c>
@@ -1602,7 +1618,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>229</v>
       </c>
@@ -1628,7 +1644,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>232</v>
       </c>
@@ -1657,7 +1673,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>232</v>
       </c>
@@ -1683,7 +1699,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -1712,7 +1728,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>231</v>
       </c>
@@ -1738,7 +1754,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1767,7 +1783,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1796,7 +1812,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1825,7 +1841,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1854,7 +1870,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1883,7 +1899,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1912,7 +1928,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1941,7 +1957,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1970,7 +1986,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -1999,7 +2015,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>187</v>
       </c>
@@ -2028,7 +2044,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>188</v>
       </c>
@@ -2057,7 +2073,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>188</v>
       </c>
@@ -2086,7 +2102,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -2115,7 +2131,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -2144,7 +2160,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -2173,7 +2189,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>190</v>
       </c>
@@ -2202,7 +2218,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>191</v>
       </c>
@@ -2231,7 +2247,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -2260,7 +2276,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -2294,8 +2310,11 @@
       <c r="K40" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -2323,8 +2342,11 @@
       <c r="K41" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2358,8 +2380,11 @@
       <c r="K42" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -2387,8 +2412,11 @@
       <c r="K43" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>184</v>
       </c>
@@ -2419,8 +2447,11 @@
       <c r="K44" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>184</v>
       </c>
@@ -2448,8 +2479,11 @@
       <c r="K45" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -2478,7 +2512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2507,7 +2541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2536,7 +2570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2565,7 +2599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -2594,7 +2628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -2623,7 +2657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -2652,7 +2686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -2681,7 +2715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -2710,7 +2744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -2739,7 +2773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>84</v>
       </c>
@@ -2768,7 +2802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -2797,7 +2831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -2826,7 +2860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -2855,7 +2889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -2884,7 +2918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -2913,7 +2947,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -2942,7 +2976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -2971,7 +3005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -3000,7 +3034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -3029,7 +3063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -3064,7 +3098,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>54</v>
       </c>
@@ -3099,7 +3133,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -3134,7 +3168,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -3169,7 +3203,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3204,7 +3238,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3239,7 +3273,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -3274,7 +3308,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -3309,7 +3343,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>194</v>
       </c>
@@ -3338,7 +3372,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>194</v>
       </c>
@@ -3367,7 +3401,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>195</v>
       </c>
@@ -3396,7 +3430,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -3425,7 +3459,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -3454,7 +3488,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>196</v>
       </c>
@@ -3483,7 +3517,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>197</v>
       </c>
@@ -3512,7 +3546,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>197</v>
       </c>
@@ -3541,7 +3575,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>198</v>
       </c>
@@ -3570,7 +3604,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>198</v>
       </c>
@@ -3599,7 +3633,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -3634,7 +3668,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -3669,7 +3703,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -3704,7 +3738,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -3739,7 +3773,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -3774,7 +3808,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -3809,7 +3843,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -3844,7 +3878,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -3879,7 +3913,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -3908,7 +3942,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>199</v>
       </c>
@@ -3943,7 +3977,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>200</v>
       </c>
@@ -3972,7 +4006,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>200</v>
       </c>
@@ -4007,7 +4041,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -4036,7 +4070,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>203</v>
       </c>
@@ -4065,7 +4099,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>204</v>
       </c>
@@ -4094,7 +4128,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>204</v>
       </c>
@@ -4123,7 +4157,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>249</v>
       </c>
@@ -4152,7 +4186,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>249</v>
       </c>
@@ -4181,7 +4215,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>205</v>
       </c>
@@ -4210,7 +4244,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -4239,7 +4273,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>206</v>
       </c>
@@ -4268,7 +4302,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -4297,7 +4331,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -4332,7 +4366,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -4367,7 +4401,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -4402,7 +4436,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -4431,7 +4465,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -4466,7 +4500,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -4501,7 +4535,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -4536,7 +4570,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -4571,7 +4605,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -4606,7 +4640,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -4641,7 +4675,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -4664,7 +4698,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>39</v>
       </c>
@@ -4699,7 +4733,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>39</v>
       </c>
@@ -4734,7 +4768,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>207</v>
       </c>
@@ -4763,7 +4797,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>207</v>
       </c>
@@ -4792,7 +4826,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>208</v>
       </c>
@@ -4821,7 +4855,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>208</v>
       </c>
@@ -4850,7 +4884,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>209</v>
       </c>
@@ -4879,7 +4913,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>209</v>
       </c>
@@ -4908,7 +4942,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>210</v>
       </c>
@@ -4937,7 +4971,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>210</v>
       </c>
@@ -4966,7 +5000,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>211</v>
       </c>
@@ -4995,7 +5029,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>211</v>
       </c>
@@ -5024,7 +5058,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>70</v>
       </c>
@@ -5053,7 +5087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>70</v>
       </c>
@@ -5082,7 +5116,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>69</v>
       </c>
@@ -5111,7 +5145,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>69</v>
       </c>
@@ -5140,7 +5174,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>71</v>
       </c>
@@ -5169,7 +5203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>71</v>
       </c>
@@ -5198,7 +5232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>72</v>
       </c>
@@ -5227,7 +5261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>72</v>
       </c>
@@ -5256,7 +5290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>40</v>
       </c>
@@ -5291,7 +5325,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>40</v>
       </c>
@@ -5326,7 +5360,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>38</v>
       </c>
@@ -5361,7 +5395,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>38</v>
       </c>
@@ -5396,7 +5430,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>37</v>
       </c>
@@ -5431,7 +5465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>37</v>
       </c>
@@ -5460,7 +5494,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>36</v>
       </c>
@@ -5495,7 +5529,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>36</v>
       </c>
@@ -5530,7 +5564,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>212</v>
       </c>
@@ -5559,7 +5593,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>212</v>
       </c>
@@ -5588,7 +5622,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>213</v>
       </c>
@@ -5617,7 +5651,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>213</v>
       </c>
@@ -5646,7 +5680,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>214</v>
       </c>
@@ -5675,7 +5709,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>214</v>
       </c>
@@ -5704,7 +5738,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>215</v>
       </c>
@@ -5733,7 +5767,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>215</v>
       </c>
@@ -5762,7 +5796,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>216</v>
       </c>
@@ -5791,7 +5825,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>216</v>
       </c>
@@ -5820,7 +5854,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>117</v>
       </c>
@@ -5849,7 +5883,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>117</v>
       </c>
@@ -5878,7 +5912,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>116</v>
       </c>
@@ -5907,7 +5941,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>116</v>
       </c>
@@ -5936,7 +5970,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>119</v>
       </c>
@@ -5965,7 +5999,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>119</v>
       </c>
@@ -5994,7 +6028,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>118</v>
       </c>
@@ -6023,7 +6057,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>118</v>
       </c>
@@ -6052,7 +6086,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>234</v>
       </c>
@@ -6081,7 +6115,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>234</v>
       </c>
@@ -6107,7 +6141,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>233</v>
       </c>
@@ -6136,7 +6170,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>233</v>
       </c>
@@ -6162,7 +6196,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>236</v>
       </c>
@@ -6191,7 +6225,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>236</v>
       </c>
@@ -6217,7 +6251,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>235</v>
       </c>
@@ -6246,7 +6280,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>235</v>
       </c>
@@ -6272,7 +6306,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>238</v>
       </c>
@@ -6301,7 +6335,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>238</v>
       </c>
@@ -6327,7 +6361,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>121</v>
       </c>
@@ -6356,7 +6390,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>121</v>
       </c>
@@ -6385,7 +6419,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>120</v>
       </c>
@@ -6414,7 +6448,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>120</v>
       </c>
@@ -6443,7 +6477,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>123</v>
       </c>
@@ -6472,7 +6506,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>123</v>
       </c>
@@ -6501,7 +6535,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>122</v>
       </c>
@@ -6530,7 +6564,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>122</v>
       </c>
@@ -6559,7 +6593,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>237</v>
       </c>
@@ -6588,7 +6622,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>237</v>
       </c>
@@ -6614,7 +6648,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>247</v>
       </c>
@@ -6643,7 +6677,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>247</v>
       </c>
@@ -6669,7 +6703,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>246</v>
       </c>
@@ -6698,7 +6732,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>246</v>
       </c>
@@ -6724,7 +6758,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>250</v>
       </c>
@@ -6753,7 +6787,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>250</v>
       </c>
@@ -6779,7 +6813,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>251</v>
       </c>
@@ -6808,7 +6842,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>251</v>
       </c>
@@ -6834,7 +6868,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>125</v>
       </c>
@@ -6863,7 +6897,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>125</v>
       </c>
@@ -6892,7 +6926,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>124</v>
       </c>
@@ -6921,7 +6955,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>124</v>
       </c>
@@ -6950,7 +6984,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>127</v>
       </c>
@@ -6979,7 +7013,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>127</v>
       </c>
@@ -7008,7 +7042,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>126</v>
       </c>
@@ -7037,7 +7071,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>126</v>
       </c>
@@ -7066,7 +7100,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>240</v>
       </c>
@@ -7095,7 +7129,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>240</v>
       </c>
@@ -7121,7 +7155,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>239</v>
       </c>
@@ -7150,7 +7184,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>239</v>
       </c>
@@ -7176,7 +7210,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>242</v>
       </c>
@@ -7205,7 +7239,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>242</v>
       </c>
@@ -7231,7 +7265,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>241</v>
       </c>
@@ -7260,7 +7294,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>241</v>
       </c>
@@ -7286,7 +7320,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="207" spans="1:11">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>252</v>
       </c>
@@ -7315,7 +7349,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="208" spans="1:11">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>252</v>
       </c>
@@ -7341,7 +7375,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>129</v>
       </c>
@@ -7370,7 +7404,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>129</v>
       </c>
@@ -7399,7 +7433,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>128</v>
       </c>
@@ -7428,7 +7462,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>128</v>
       </c>
@@ -7457,7 +7491,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>131</v>
       </c>
@@ -7486,7 +7520,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>131</v>
       </c>
@@ -7515,7 +7549,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>130</v>
       </c>
@@ -7544,7 +7578,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>130</v>
       </c>
@@ -7573,7 +7607,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>243</v>
       </c>
@@ -7602,7 +7636,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>243</v>
       </c>
@@ -7628,7 +7662,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>248</v>
       </c>
@@ -7657,7 +7691,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>248</v>
       </c>
@@ -7683,7 +7717,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>244</v>
       </c>
@@ -7712,7 +7746,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>244</v>
       </c>
@@ -7741,7 +7775,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>245</v>
       </c>
@@ -7770,7 +7804,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>245</v>
       </c>
@@ -7796,7 +7830,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>228</v>
       </c>
@@ -7825,7 +7859,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>228</v>
       </c>
@@ -7851,7 +7885,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>35</v>
       </c>
@@ -7886,7 +7920,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>74</v>
       </c>
@@ -7915,7 +7949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>74</v>
       </c>
@@ -7944,7 +7978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>73</v>
       </c>
@@ -7973,7 +8007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>73</v>
       </c>
@@ -8002,7 +8036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:11">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>109</v>
       </c>
@@ -8031,7 +8065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="233" spans="1:11">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>109</v>
       </c>
@@ -8060,7 +8094,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>68</v>
       </c>
@@ -8089,7 +8123,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>68</v>
       </c>
@@ -8118,7 +8152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="236" spans="1:11">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>66</v>
       </c>
@@ -8147,7 +8181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="237" spans="1:11">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>66</v>
       </c>
@@ -8176,7 +8210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>67</v>
       </c>
@@ -8205,7 +8239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>67</v>
       </c>
@@ -8234,7 +8268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="240" spans="1:11">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>63</v>
       </c>
@@ -8263,7 +8297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="241" spans="1:11">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>63</v>
       </c>
@@ -8292,7 +8326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="242" spans="1:11">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>64</v>
       </c>
@@ -8321,7 +8355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>64</v>
       </c>
@@ -8350,7 +8384,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>174</v>
       </c>
@@ -8384,8 +8418,11 @@
       <c r="K244" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="245" spans="1:11">
+      <c r="L244" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>174</v>
       </c>
@@ -8419,8 +8456,11 @@
       <c r="K245" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="246" spans="1:11">
+      <c r="L245" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>168</v>
       </c>
@@ -8454,8 +8494,11 @@
       <c r="K246" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="247" spans="1:11">
+      <c r="L246" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>168</v>
       </c>
@@ -8489,8 +8532,11 @@
       <c r="K247" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="248" spans="1:11">
+      <c r="L247" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>55</v>
       </c>
@@ -8524,8 +8570,11 @@
       <c r="K248" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="249" spans="1:11">
+      <c r="L248" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>55</v>
       </c>
@@ -8559,8 +8608,11 @@
       <c r="K249" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="250" spans="1:11">
+      <c r="L249" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>170</v>
       </c>
@@ -8594,8 +8646,11 @@
       <c r="K250" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="251" spans="1:11">
+      <c r="L250" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>170</v>
       </c>
@@ -8629,8 +8684,11 @@
       <c r="K251" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="252" spans="1:11">
+      <c r="L251" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>165</v>
       </c>
@@ -8664,8 +8722,11 @@
       <c r="K252" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="253" spans="1:11">
+      <c r="L252" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>165</v>
       </c>
@@ -8699,8 +8760,11 @@
       <c r="K253" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="254" spans="1:11">
+      <c r="L253" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>172</v>
       </c>
@@ -8734,8 +8798,11 @@
       <c r="K254" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="255" spans="1:11">
+      <c r="L254" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>172</v>
       </c>
@@ -8769,8 +8836,11 @@
       <c r="K255" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="256" spans="1:11">
+      <c r="L255" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>34</v>
       </c>
@@ -8804,8 +8874,11 @@
       <c r="K256" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="257" spans="1:11">
+      <c r="L256" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>34</v>
       </c>
@@ -8839,8 +8912,11 @@
       <c r="K257" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="258" spans="1:11">
+      <c r="L257" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>140</v>
       </c>
@@ -8874,8 +8950,11 @@
       <c r="K258" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="259" spans="1:11">
+      <c r="L258" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>140</v>
       </c>
@@ -8909,8 +8988,11 @@
       <c r="K259" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="260" spans="1:11">
+      <c r="L259" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>32</v>
       </c>
@@ -8944,8 +9026,11 @@
       <c r="K260" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="261" spans="1:11">
+      <c r="L260" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>32</v>
       </c>
@@ -8979,8 +9064,11 @@
       <c r="K261" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="262" spans="1:11">
+      <c r="L261" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>138</v>
       </c>
@@ -9002,8 +9090,11 @@
       <c r="K262" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="263" spans="1:11">
+      <c r="L262" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>33</v>
       </c>
@@ -9037,8 +9128,11 @@
       <c r="K263" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="264" spans="1:11">
+      <c r="L263" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>33</v>
       </c>
@@ -9072,8 +9166,11 @@
       <c r="K264" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="265" spans="1:11">
+      <c r="L264" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>30</v>
       </c>
@@ -9107,8 +9204,11 @@
       <c r="K265" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="266" spans="1:11">
+      <c r="L265" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>30</v>
       </c>
@@ -9142,8 +9242,11 @@
       <c r="K266" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="267" spans="1:11">
+      <c r="L266" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>31</v>
       </c>
@@ -9177,8 +9280,11 @@
       <c r="K267" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="268" spans="1:11">
+      <c r="L267" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>31</v>
       </c>
@@ -9212,8 +9318,11 @@
       <c r="K268" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="269" spans="1:11">
+      <c r="L268" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>23</v>
       </c>
@@ -9247,8 +9356,11 @@
       <c r="K269" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="270" spans="1:11">
+      <c r="L269" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>23</v>
       </c>
@@ -9282,8 +9394,11 @@
       <c r="K270" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="271" spans="1:11">
+      <c r="L270" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>29</v>
       </c>
@@ -9317,8 +9432,11 @@
       <c r="K271" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="272" spans="1:11">
+      <c r="L271" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>29</v>
       </c>
@@ -9352,8 +9470,11 @@
       <c r="K272" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="273" spans="1:11">
+      <c r="L272" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>155</v>
       </c>
@@ -9381,8 +9502,11 @@
       <c r="K273" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="274" spans="1:11">
+      <c r="L273" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>155</v>
       </c>
@@ -9416,8 +9540,11 @@
       <c r="K274" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="275" spans="1:11">
+      <c r="L274" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>154</v>
       </c>
@@ -9445,8 +9572,11 @@
       <c r="K275" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="276" spans="1:11">
+      <c r="L275" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>154</v>
       </c>
@@ -9480,8 +9610,11 @@
       <c r="K276" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="277" spans="1:11">
+      <c r="L276" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>153</v>
       </c>
@@ -9515,8 +9648,11 @@
       <c r="K277" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="278" spans="1:11">
+      <c r="L277" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>153</v>
       </c>
@@ -9550,8 +9686,11 @@
       <c r="K278" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="279" spans="1:11">
+      <c r="L278" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>151</v>
       </c>
@@ -9579,8 +9718,11 @@
       <c r="K279" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="280" spans="1:11">
+      <c r="L279" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>151</v>
       </c>
@@ -9608,8 +9750,11 @@
       <c r="K280" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="281" spans="1:11">
+      <c r="L280" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>159</v>
       </c>
@@ -9637,8 +9782,11 @@
       <c r="K281" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="282" spans="1:11">
+      <c r="L281" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>159</v>
       </c>
@@ -9672,8 +9820,11 @@
       <c r="K282" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="283" spans="1:11">
+      <c r="L282" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>28</v>
       </c>
@@ -9701,8 +9852,11 @@
       <c r="K283" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="284" spans="1:11">
+      <c r="L283" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>28</v>
       </c>
@@ -9736,8 +9890,11 @@
       <c r="K284" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="285" spans="1:11">
+      <c r="L284" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>27</v>
       </c>
@@ -9765,8 +9922,11 @@
       <c r="K285" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="286" spans="1:11">
+      <c r="L285" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>27</v>
       </c>
@@ -9800,8 +9960,11 @@
       <c r="K286" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="287" spans="1:11">
+      <c r="L286" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>149</v>
       </c>
@@ -9829,8 +9992,11 @@
       <c r="K287" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="288" spans="1:11">
+      <c r="L287" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>149</v>
       </c>
@@ -9864,8 +10030,11 @@
       <c r="K288" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="289" spans="1:11">
+      <c r="L288" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>163</v>
       </c>
@@ -9893,8 +10062,11 @@
       <c r="K289" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="290" spans="1:11">
+      <c r="L289" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>163</v>
       </c>
@@ -9928,8 +10100,11 @@
       <c r="K290" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="291" spans="1:11">
+      <c r="L290" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>145</v>
       </c>
@@ -9957,8 +10132,11 @@
       <c r="K291" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="292" spans="1:11">
+      <c r="L291" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>145</v>
       </c>
@@ -9992,8 +10170,11 @@
       <c r="K292" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="293" spans="1:11">
+      <c r="L292" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>161</v>
       </c>
@@ -10021,8 +10202,11 @@
       <c r="K293" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="294" spans="1:11">
+      <c r="L293" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>161</v>
       </c>
@@ -10056,8 +10240,11 @@
       <c r="K294" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="295" spans="1:11">
+      <c r="L294" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>144</v>
       </c>
@@ -10085,8 +10272,11 @@
       <c r="K295" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="296" spans="1:11">
+      <c r="L295" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>144</v>
       </c>
@@ -10120,8 +10310,11 @@
       <c r="K296" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="297" spans="1:11">
+      <c r="L296" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>59</v>
       </c>
@@ -10150,7 +10343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="298" spans="1:11">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>59</v>
       </c>
@@ -10179,7 +10372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="299" spans="1:11">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>185</v>
       </c>
@@ -10193,7 +10386,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="300" spans="1:11">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>26</v>
       </c>
@@ -10227,8 +10420,11 @@
       <c r="K300" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="301" spans="1:11">
+      <c r="L300" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>26</v>
       </c>
@@ -10262,8 +10458,11 @@
       <c r="K301" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="302" spans="1:11">
+      <c r="L301" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>22</v>
       </c>
@@ -10297,8 +10496,11 @@
       <c r="K302" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="303" spans="1:11">
+      <c r="L302" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>22</v>
       </c>
@@ -10332,8 +10534,11 @@
       <c r="K303" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="304" spans="1:11">
+      <c r="L303" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>25</v>
       </c>
@@ -10367,8 +10572,11 @@
       <c r="K304" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="305" spans="1:11">
+      <c r="L304" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>25</v>
       </c>
@@ -10402,8 +10610,11 @@
       <c r="K305" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="306" spans="1:11">
+      <c r="L305" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>24</v>
       </c>
@@ -10431,8 +10642,11 @@
       <c r="K306" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="307" spans="1:11">
+      <c r="L306" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>52</v>
       </c>
@@ -10466,8 +10680,11 @@
       <c r="K307" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="308" spans="1:11">
+      <c r="L307" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>53</v>
       </c>
@@ -10501,8 +10718,11 @@
       <c r="K308" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="309" spans="1:11">
+      <c r="L308" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>103</v>
       </c>
@@ -10531,7 +10751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="310" spans="1:11">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>103</v>
       </c>
@@ -10560,7 +10780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="311" spans="1:11">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>102</v>
       </c>
@@ -10589,7 +10809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="312" spans="1:11">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>102</v>
       </c>
@@ -10618,7 +10838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="313" spans="1:11">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>101</v>
       </c>
@@ -10647,7 +10867,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="314" spans="1:11">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>101</v>
       </c>
@@ -10676,7 +10896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="315" spans="1:11">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>99</v>
       </c>
@@ -10705,7 +10925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="316" spans="1:11">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>99</v>
       </c>
@@ -10734,7 +10954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="317" spans="1:11">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>100</v>
       </c>
@@ -10763,7 +10983,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="318" spans="1:11">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>100</v>
       </c>
@@ -10792,7 +11012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="319" spans="1:11">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>98</v>
       </c>
@@ -10821,7 +11041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="320" spans="1:11">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>98</v>
       </c>
@@ -10850,7 +11070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="321" spans="1:11">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>110</v>
       </c>
@@ -10879,7 +11099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="322" spans="1:11">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>110</v>
       </c>
@@ -10908,7 +11128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="323" spans="1:11">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>105</v>
       </c>
@@ -10937,7 +11157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="324" spans="1:11">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>105</v>
       </c>
@@ -10966,7 +11186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="325" spans="1:11">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>107</v>
       </c>
@@ -10995,7 +11215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="326" spans="1:11">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>107</v>
       </c>
@@ -11024,7 +11244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="327" spans="1:11">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>106</v>
       </c>
@@ -11059,7 +11279,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="328" spans="1:11">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>106</v>
       </c>
@@ -11088,7 +11308,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="329" spans="1:11">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>108</v>
       </c>
@@ -11123,7 +11343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="330" spans="1:11">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>108</v>
       </c>
@@ -11152,7 +11372,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="331" spans="1:11">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>80</v>
       </c>
@@ -11181,7 +11401,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="332" spans="1:11">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>80</v>
       </c>
@@ -11210,7 +11430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="333" spans="1:11">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>92</v>
       </c>
@@ -11239,7 +11459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="334" spans="1:11">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>92</v>
       </c>
@@ -11268,7 +11488,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="335" spans="1:11">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>96</v>
       </c>
@@ -11297,7 +11517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="336" spans="1:11">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>96</v>
       </c>
@@ -11326,7 +11546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="337" spans="1:11">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>95</v>
       </c>
@@ -11355,7 +11575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="338" spans="1:11">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>95</v>
       </c>
@@ -11384,7 +11604,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="339" spans="1:11">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>93</v>
       </c>
@@ -11413,7 +11633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="340" spans="1:11">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>93</v>
       </c>
@@ -11442,7 +11662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="341" spans="1:11">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>104</v>
       </c>
@@ -11471,7 +11691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="342" spans="1:11">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>104</v>
       </c>
@@ -11500,7 +11720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="343" spans="1:11">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>97</v>
       </c>
@@ -11529,7 +11749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="344" spans="1:11">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>97</v>
       </c>
@@ -11558,7 +11778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="345" spans="1:11">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>94</v>
       </c>
@@ -11587,7 +11807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="346" spans="1:11">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>94</v>
       </c>
@@ -11616,7 +11836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="347" spans="1:11">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>58</v>
       </c>
@@ -11645,7 +11865,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="348" spans="1:11">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>58</v>
       </c>
@@ -11674,7 +11894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="349" spans="1:11">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>56</v>
       </c>
@@ -11703,7 +11923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="350" spans="1:11">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>56</v>
       </c>
@@ -11732,7 +11952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="351" spans="1:11">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>51</v>
       </c>
@@ -11767,7 +11987,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="352" spans="1:11">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>50</v>
       </c>
@@ -11790,7 +12010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="353" spans="1:11">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>49</v>
       </c>
@@ -11813,7 +12033,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="354" spans="1:11">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>48</v>
       </c>
@@ -11836,7 +12056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="355" spans="1:11">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>47</v>
       </c>
@@ -11859,7 +12079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="356" spans="1:11">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>223</v>
       </c>
@@ -11894,7 +12114,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="357" spans="1:11">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>60</v>
       </c>
@@ -11923,7 +12143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="358" spans="1:11">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>60</v>
       </c>
@@ -11952,7 +12172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="359" spans="1:11">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>62</v>
       </c>
@@ -11981,7 +12201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="360" spans="1:11">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>62</v>
       </c>
@@ -12010,7 +12230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="361" spans="1:11">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>75</v>
       </c>
@@ -12039,7 +12259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="362" spans="1:11">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>75</v>
       </c>
@@ -12068,7 +12288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="363" spans="1:11">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>76</v>
       </c>
@@ -12097,7 +12317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="364" spans="1:11">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>76</v>
       </c>
@@ -12126,7 +12346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="365" spans="1:11">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>77</v>
       </c>
@@ -12155,7 +12375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="366" spans="1:11">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>77</v>
       </c>
@@ -12184,7 +12404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="367" spans="1:11">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>78</v>
       </c>
@@ -12213,7 +12433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="368" spans="1:11">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>78</v>
       </c>
@@ -12242,7 +12462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="369" spans="1:11">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>111</v>
       </c>
@@ -12271,7 +12491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="370" spans="1:11">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>111</v>
       </c>
@@ -12300,7 +12520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="371" spans="1:11">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>46</v>
       </c>
@@ -12335,7 +12555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="372" spans="1:11">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>45</v>
       </c>
@@ -12364,7 +12584,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="373" spans="1:11">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>82</v>
       </c>
@@ -12393,7 +12613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="374" spans="1:11">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>82</v>
       </c>
@@ -12422,7 +12642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="375" spans="1:11">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>65</v>
       </c>
@@ -12451,7 +12671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="376" spans="1:11">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>65</v>
       </c>

</xml_diff>